<commit_message>
Changed Names of the h2b files, the models aren't hardcoded anymore, now you can switch back to the first song while playing the second one.
</commit_message>
<xml_diff>
--- a/Project Rubric.xlsx
+++ b/Project Rubric.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Desktop\DEV4 Project Repo\DEV4-LevelRenderer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Desktop\DEV4-LevelRenderer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8B2ADAB-FB36-40B2-BD1D-07E9300D86BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD264DC-6A0D-4A80-BAB8-8E8FDB152F21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
   </bookViews>
@@ -1722,8 +1722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A40538-A3BB-461B-BC01-A04BD38DD6FA}">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1773,7 +1773,7 @@
         <v>0.05</v>
       </c>
       <c r="C4" s="3">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1784,7 +1784,7 @@
         <v>0.01</v>
       </c>
       <c r="C5" s="3">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1795,7 +1795,7 @@
         <v>0.01</v>
       </c>
       <c r="C6" s="3">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1806,7 +1806,7 @@
         <v>0.1</v>
       </c>
       <c r="C7" s="3">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1828,7 +1828,7 @@
         <v>0.1</v>
       </c>
       <c r="C9" s="3">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1863,7 +1863,7 @@
       </c>
       <c r="C12" s="6">
         <f>SUM(C2:C11)</f>
-        <v>0.35000000000000003</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
@@ -2265,7 +2265,7 @@
       </c>
       <c r="C48" s="17">
         <f>MIN(SUM(C47,C42,C26,C12),100%)</f>
-        <v>0.41000000000000003</v>
+        <v>0.19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Triangulated all of my models and changed the h2b files. Also deleted the mtl files from the repo and made some small edits to the ReadMe and the rubric
</commit_message>
<xml_diff>
--- a/Project Rubric.xlsx
+++ b/Project Rubric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Desktop\DEV4-LevelRenderer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD264DC-6A0D-4A80-BAB8-8E8FDB152F21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E508EF-332A-4F05-9819-066A327D2418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
   </bookViews>
@@ -1722,8 +1722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A40538-A3BB-461B-BC01-A04BD38DD6FA}">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1773,7 +1773,7 @@
         <v>0.05</v>
       </c>
       <c r="C4" s="3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1784,7 +1784,7 @@
         <v>0.01</v>
       </c>
       <c r="C5" s="3">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1795,7 +1795,7 @@
         <v>0.01</v>
       </c>
       <c r="C6" s="3">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1806,7 +1806,7 @@
         <v>0.1</v>
       </c>
       <c r="C7" s="3">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1828,7 +1828,7 @@
         <v>0.1</v>
       </c>
       <c r="C9" s="3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1863,7 +1863,7 @@
       </c>
       <c r="C12" s="6">
         <f>SUM(C2:C11)</f>
-        <v>0.13</v>
+        <v>0.35000000000000003</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
@@ -2265,7 +2265,7 @@
       </c>
       <c r="C48" s="17">
         <f>MIN(SUM(C47,C42,C26,C12),100%)</f>
-        <v>0.19</v>
+        <v>0.41000000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Models are rendering on the right position, scale, and rotation. Only colors remain now. Also, made the repo a little more organized and added the objs
</commit_message>
<xml_diff>
--- a/Project Rubric.xlsx
+++ b/Project Rubric.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Desktop\DEV4-LevelRenderer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E508EF-332A-4F05-9819-066A327D2418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28FCAA8-EA6F-4DC3-B591-449A980F504D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1722,8 +1722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A40538-A3BB-461B-BC01-A04BD38DD6FA}">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1817,7 +1817,7 @@
         <v>0.1</v>
       </c>
       <c r="C8" s="3">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1828,7 +1828,7 @@
         <v>0.1</v>
       </c>
       <c r="C9" s="3">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1863,7 +1863,7 @@
       </c>
       <c r="C12" s="6">
         <f>SUM(C2:C11)</f>
-        <v>0.35000000000000003</v>
+        <v>0.40000000000000008</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
@@ -2265,7 +2265,7 @@
       </c>
       <c r="C48" s="17">
         <f>MIN(SUM(C47,C42,C26,C12),100%)</f>
-        <v>0.41000000000000003</v>
+        <v>0.46000000000000008</v>
       </c>
     </row>
   </sheetData>

</xml_diff>